<commit_message>
Actualilzación de dashboard en excel
</commit_message>
<xml_diff>
--- a/data/dashboard_finanzas.xlsx
+++ b/data/dashboard_finanzas.xlsx
@@ -8,19 +8,41 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Curso Python\DataScience\finanzas-dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448E2F42-74B6-4CC4-B572-BFA8C8E83D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3E1EFB-48A6-441E-AA8A-ADED5EB4C127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="finanzas" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="3" r:id="rId1"/>
+    <sheet name="finanzas" sheetId="1" r:id="rId2"/>
+    <sheet name="Dashboard" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="SegmentaciónDeDatos_Categoria">#N/A</definedName>
+    <definedName name="SegmentaciónDeDatos_Fecha">#N/A</definedName>
+    <definedName name="SegmentaciónDeDatos_Tipo">#N/A</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="9" r:id="rId4"/>
+  </pivotCaches>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
+      <x14:slicerCaches>
+        <x14:slicerCache r:id="rId5"/>
+        <x14:slicerCache r:id="rId6"/>
+        <x14:slicerCache r:id="rId7"/>
+      </x14:slicerCaches>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="29">
   <si>
     <t>Fecha</t>
   </si>
@@ -86,6 +108,27 @@
   </si>
   <si>
     <t>Cuya</t>
+  </si>
+  <si>
+    <t>Etiquetas de fila</t>
+  </si>
+  <si>
+    <t>Total general</t>
+  </si>
+  <si>
+    <t>(Todas)</t>
+  </si>
+  <si>
+    <t>Etiquetas de columna</t>
+  </si>
+  <si>
+    <t>Suma de Monto</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>jul</t>
   </si>
 </sst>
 </file>
@@ -569,7 +612,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -577,6 +620,11 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -633,6 +681,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF93FFC4"/>
+      <color rgb="FFFF8181"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -642,6 +696,3951 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[dashboard_finanzas.xlsx]Hoja2!TablaDinámica1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+          <a:sp3d contourW="25400">
+            <a:contourClr>
+              <a:schemeClr val="lt1"/>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja2!$A$4:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Alimentacion</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Guardado</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ingreso Semanal</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Pago</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Parqueadero</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Salario</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Transporte</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$B$4:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>18500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1B30-480C-8C64-EA09B715497F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[dashboard_finanzas.xlsx]Hoja2!TablaDinámica2</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="FF8181"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="93FFC4"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$E$1:$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Egreso</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF8181"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Hoja2!$D$3:$D$5</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="1"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>jul</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2025</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$E$3:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>28500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A2C8-4561-B0BC-EC6E3F13C26F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$F$1:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ingreso</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="93FFC4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Hoja2!$D$3:$D$5</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="1"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>jul</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2025</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$F$3:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>442500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-A2C8-4561-B0BC-EC6E3F13C26F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1508426255"/>
+        <c:axId val="1338619743"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1508426255"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1338619743"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1338619743"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1508426255"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[dashboard_finanzas.xlsx]Hoja2!TablaDinámica3</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Hoja2!$I$4:$I$6</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="1"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>jul</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2025</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$J$4:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>471000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E06B-47E2-8E4F-5757AF444DAD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1510252815"/>
+        <c:axId val="1510254479"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1510252815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1510254479"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1510254479"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1510252815"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="262">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1066800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23C69F92-4A4D-4FBD-816D-547405D6DA2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A6D80C1-4F43-4244-8F0D-D7C5CAE0199A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>437303</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>88053</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>246380</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>88053</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B878FD4-65F2-480A-A9A7-CEF0440FA532}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>276860</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>119804</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>52493</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>67946</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="14" name="Fecha">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6256EA0-D199-4A9A-976D-28ADCD705CD1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Fecha"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4065693" y="5517304"/>
+              <a:ext cx="1828800" cy="2466975"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100"/>
+                <a:t>Esta forma representa una segmentación de datos. La segmentación de datos se admite en Excel 2010 y versiones posteriores.
+Si la forma se modificó en una versión anterior de Excel o si el libro se guardó en Excel 2003 o una versión anterior, no se puede usar la segmentación de datos.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>143086</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>134197</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>627803</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>82339</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="15" name="Categoria">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EE3CA5C-00BA-46F8-81D3-2DE55F887DD1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Categoria"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5985086" y="5531697"/>
+              <a:ext cx="1828800" cy="2466975"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100"/>
+                <a:t>Esta forma representa una segmentación de datos. La segmentación de datos se admite en Excel 2010 y versiones posteriores.
+Si la forma se modificó en una versión anterior de Excel o si el libro se guardó en Excel 2003 o una versión anterior, no se puede usar la segmentación de datos.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>771314</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>127424</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>398780</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>75566</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="16" name="Tipo">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17AB7781-136A-4EF1-9E8D-E3D72F485C2C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Tipo"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7957397" y="5524924"/>
+              <a:ext cx="1828800" cy="2466975"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-CO" sz="1100"/>
+                <a:t>Esta forma representa una segmentación de datos. La segmentación de datos se admite en Excel 2010 y versiones posteriores.
+Si la forma se modificó en una versión anterior de Excel o si el libro se guardó en Excel 2003 o una versión anterior, no se puede usar la segmentación de datos.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="USER" refreshedDate="45841.852184374999" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="8" xr:uid="{BEC3C783-8187-431C-B899-F77816A98D6D}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Finanzas"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="Fecha" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2025-07-01T00:00:00" maxDate="2025-07-04T00:00:00" count="3">
+        <d v="2025-07-01T00:00:00"/>
+        <d v="2025-07-02T00:00:00"/>
+        <d v="2025-07-03T00:00:00"/>
+      </sharedItems>
+      <fieldGroup par="5" base="0">
+        <rangePr groupBy="months" startDate="2025-07-01T00:00:00" endDate="2025-07-04T00:00:00"/>
+        <groupItems count="14">
+          <s v="&lt;1/07/2025"/>
+          <s v="ene"/>
+          <s v="feb"/>
+          <s v="mar"/>
+          <s v="abr"/>
+          <s v="may"/>
+          <s v="jun"/>
+          <s v="jul"/>
+          <s v="ago"/>
+          <s v="sep"/>
+          <s v="oct"/>
+          <s v="nov"/>
+          <s v="dic"/>
+          <s v="&gt;4/07/2025"/>
+        </groupItems>
+      </fieldGroup>
+    </cacheField>
+    <cacheField name="Categoria" numFmtId="0">
+      <sharedItems count="7">
+        <s v="Guardado"/>
+        <s v="Ingreso Semanal"/>
+        <s v="Alimentacion"/>
+        <s v="Pago"/>
+        <s v="Transporte"/>
+        <s v="Salario"/>
+        <s v="Parqueadero"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Descripcion" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Monto" numFmtId="3">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2000" maxValue="200000" count="7">
+        <n v="180000"/>
+        <n v="60000"/>
+        <n v="10500"/>
+        <n v="8000"/>
+        <n v="2500"/>
+        <n v="200000"/>
+        <n v="2000"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Tipo" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Ingreso"/>
+        <s v="Egreso"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Años" numFmtId="0" databaseField="0">
+      <fieldGroup base="0">
+        <rangePr groupBy="years" startDate="2025-07-01T00:00:00" endDate="2025-07-04T00:00:00"/>
+        <groupItems count="3">
+          <s v="&lt;1/07/2025"/>
+          <s v="2025"/>
+          <s v="&gt;4/07/2025"/>
+        </groupItems>
+      </fieldGroup>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition pivotCacheId="1038291983"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="8">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Ahorros anteriores"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="Apoyo Padre"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="Almuerzo"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Desayuno"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <s v="Manuel Hernandez"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <s v="Nuevos tornillos para los handsavers"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <s v="Pago Centro de Desarrollo"/>
+    <x v="5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="6"/>
+    <s v="Cuya"/>
+    <x v="6"/>
+    <x v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C1555650-2751-4973-B725-06D328F2FE7E}" name="TablaDinámica3" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="I3:J6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="6">
+    <pivotField axis="axisRow" numFmtId="14" showAll="0">
+      <items count="15">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="8">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="3" showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="5"/>
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="4" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Suma de Monto" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E6F561CE-D2C0-4395-9932-CD5D0AAA52A2}" name="TablaDinámica2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="D1:G5" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField axis="axisRow" numFmtId="14" showAll="0">
+      <items count="15">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="8">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="3" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="5"/>
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Suma de Monto" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EF513811-D5EA-4132-9D71-DA48AE7863DD}" name="TablaDinámica1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="6">
+    <pivotField numFmtId="14" showAll="0">
+      <items count="15">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="3" showAll="0">
+      <items count="8">
+        <item x="6"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="4" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Suma de Monto" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="SegmentaciónDeDatos_Fecha" xr10:uid="{EC35CE8A-8C1B-4FCC-B6AF-2984DFACF88B}" sourceName="Fecha">
+  <pivotTables>
+    <pivotTable tabId="3" name="TablaDinámica1"/>
+    <pivotTable tabId="3" name="TablaDinámica2"/>
+    <pivotTable tabId="3" name="TablaDinámica3"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1038291983">
+      <items count="14">
+        <i x="7" s="1"/>
+        <i x="1" s="1" nd="1"/>
+        <i x="2" s="1" nd="1"/>
+        <i x="3" s="1" nd="1"/>
+        <i x="4" s="1" nd="1"/>
+        <i x="5" s="1" nd="1"/>
+        <i x="6" s="1" nd="1"/>
+        <i x="8" s="1" nd="1"/>
+        <i x="9" s="1" nd="1"/>
+        <i x="10" s="1" nd="1"/>
+        <i x="11" s="1" nd="1"/>
+        <i x="12" s="1" nd="1"/>
+        <i x="0" s="1" nd="1"/>
+        <i x="13" s="1" nd="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="SegmentaciónDeDatos_Categoria" xr10:uid="{190B59E8-AAE4-4E9C-8B52-F560F0440042}" sourceName="Categoria">
+  <pivotTables>
+    <pivotTable tabId="3" name="TablaDinámica1"/>
+    <pivotTable tabId="3" name="TablaDinámica2"/>
+    <pivotTable tabId="3" name="TablaDinámica3"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1038291983">
+      <items count="7">
+        <i x="2" s="1"/>
+        <i x="0" s="1"/>
+        <i x="1" s="1"/>
+        <i x="3" s="1"/>
+        <i x="6" s="1"/>
+        <i x="5" s="1"/>
+        <i x="4" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache3.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="SegmentaciónDeDatos_Tipo" xr10:uid="{6219A759-6E3F-4D2B-AAFE-AD623615847D}" sourceName="Tipo">
+  <pivotTables>
+    <pivotTable tabId="3" name="TablaDinámica1"/>
+    <pivotTable tabId="3" name="TablaDinámica2"/>
+    <pivotTable tabId="3" name="TablaDinámica3"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1038291983">
+      <items count="2">
+        <i x="1" s="1"/>
+        <i x="0" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Fecha" xr10:uid="{52DA86D6-D1E0-4CBF-BA63-8C0108B248D1}" cache="SegmentaciónDeDatos_Fecha" caption="Fecha" rowHeight="234950"/>
+  <slicer name="Categoria" xr10:uid="{EC9DBCCF-4726-4B43-96DE-822670ABC072}" cache="SegmentaciónDeDatos_Categoria" caption="Categoria" rowHeight="234950"/>
+  <slicer name="Tipo" xr10:uid="{9FEE55AD-D736-4163-BF7E-9D38D8B0D37A}" cache="SegmentaciónDeDatos_Tipo" caption="Tipo" rowHeight="234950"/>
+</slicers>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -954,10 +4953,211 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E887D1-2AB5-49E1-8B2F-C3E88E76F043}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="5">
+        <v>28500</v>
+      </c>
+      <c r="F3" s="5">
+        <v>442500</v>
+      </c>
+      <c r="G3" s="5">
+        <v>471000</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5">
+        <v>18500</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="5">
+        <v>28500</v>
+      </c>
+      <c r="F4" s="5">
+        <v>442500</v>
+      </c>
+      <c r="G4" s="5">
+        <v>471000</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="5">
+        <v>471000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5">
+        <v>180000</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="5">
+        <v>28500</v>
+      </c>
+      <c r="F5" s="5">
+        <v>442500</v>
+      </c>
+      <c r="G5" s="5">
+        <v>471000</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="5">
+        <v>471000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5">
+        <v>60000</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="5">
+        <v>471000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="5">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="5">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="5">
+        <v>471000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId5"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -1128,4 +5328,16 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9D593E1-8731-4DCC-824D-A7026EDCC927}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Día 6: Documentación del proyecto finalizada
</commit_message>
<xml_diff>
--- a/data/dashboard_finanzas.xlsx
+++ b/data/dashboard_finanzas.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Curso Python\DataScience\finanzas-dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3E1EFB-48A6-441E-AA8A-ADED5EB4C127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBE0E90-184A-4C46-915B-7E50503A4704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
   <si>
     <t>Fecha</t>
   </si>
@@ -130,12 +130,24 @@
   <si>
     <t>jul</t>
   </si>
+  <si>
+    <t>Gráfico de Pastel por Categoria</t>
+  </si>
+  <si>
+    <t>Graficos de columnas Ingreso vs Gasto</t>
+  </si>
+  <si>
+    <t>Totales por Mes</t>
+  </si>
+  <si>
+    <t>Saldo Acumulado</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,8 +282,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -451,8 +491,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FFD9E1F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -567,6 +613,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -612,7 +676,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -626,6 +690,26 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -811,6 +895,139 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+          <a:sp3d contourW="25400">
+            <a:contourClr>
+              <a:schemeClr val="lt1"/>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+          <a:sp3d contourW="25400">
+            <a:contourClr>
+              <a:schemeClr val="lt1"/>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+          <a:sp3d contourW="25400">
+            <a:contourClr>
+              <a:schemeClr val="lt1"/>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+          <a:sp3d contourW="25400">
+            <a:contourClr>
+              <a:schemeClr val="lt1"/>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+          <a:sp3d contourW="25400">
+            <a:contourClr>
+              <a:schemeClr val="lt1"/>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+          <a:sp3d contourW="25400">
+            <a:contourClr>
+              <a:schemeClr val="lt1"/>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+          <a:sp3d contourW="25400">
+            <a:contourClr>
+              <a:schemeClr val="lt1"/>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:view3D>
       <c:rotX val="30"/>
@@ -888,6 +1105,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-E595-4071-808C-8C0BD8861FC7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -908,6 +1130,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-E595-4071-808C-8C0BD8861FC7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -928,6 +1155,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-E595-4071-808C-8C0BD8861FC7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -948,6 +1180,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-E595-4071-808C-8C0BD8861FC7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -968,6 +1205,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-E595-4071-808C-8C0BD8861FC7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -988,6 +1230,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-E595-4071-808C-8C0BD8861FC7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -1010,6 +1257,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-E595-4071-808C-8C0BD8861FC7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -3731,15 +3983,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>144780</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:colOff>328084</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>2962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1066800</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:colOff>1250104</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>2962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3766,16 +4018,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1181100</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>80010</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>175683</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>175259</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>80010</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>574040</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>175259</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3802,16 +4054,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>437303</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>88053</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>216725</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>2829</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>246380</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>88053</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>418499</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>2829</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3844,13 +4096,13 @@
       <xdr:rowOff>119804</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>52493</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>573861</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>67946</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="14" name="Fecha">
@@ -3873,7 +4125,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -3927,8 +4179,8 @@
       <xdr:row>44</xdr:row>
       <xdr:rowOff>82339</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="15" name="Categoria">
@@ -3951,7 +4203,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -4005,8 +4257,8 @@
       <xdr:row>44</xdr:row>
       <xdr:rowOff>75566</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="16" name="Tipo">
@@ -4029,7 +4281,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -4217,7 +4469,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C1555650-2751-4973-B725-06D328F2FE7E}" name="TablaDinámica3" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C1555650-2751-4973-B725-06D328F2FE7E}" name="TablaDinámica3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="I3:J6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
@@ -4317,7 +4569,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E6F561CE-D2C0-4395-9932-CD5D0AAA52A2}" name="TablaDinámica2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E6F561CE-D2C0-4395-9932-CD5D0AAA52A2}" name="TablaDinámica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="D1:G5" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
@@ -4440,7 +4692,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EF513811-D5EA-4132-9D71-DA48AE7863DD}" name="TablaDinámica1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EF513811-D5EA-4132-9D71-DA48AE7863DD}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField numFmtId="14" showAll="0">
@@ -4541,12 +4793,96 @@
   <dataFields count="1">
     <dataField name="Suma de Monto" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="8">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="6"/>
           </reference>
         </references>
       </pivotArea>
@@ -4954,10 +5290,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E887D1-2AB5-49E1-8B2F-C3E88E76F043}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:S67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="56" workbookViewId="0">
+      <selection activeCell="W75" sqref="W75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4967,11 +5303,13 @@
     <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -5140,7 +5478,120 @@
         <v>471000</v>
       </c>
     </row>
+    <row r="47" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="G47" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="N47" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="O47" s="8"/>
+      <c r="P47" s="8"/>
+      <c r="Q47" s="8"/>
+      <c r="R47" s="8"/>
+      <c r="S47" s="8"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="8"/>
+      <c r="N48" s="8"/>
+      <c r="O48" s="8"/>
+      <c r="P48" s="8"/>
+      <c r="Q48" s="8"/>
+      <c r="R48" s="8"/>
+      <c r="S48" s="8"/>
+    </row>
+    <row r="51" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P51" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q51" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P52" s="10"/>
+      <c r="Q52" s="10"/>
+    </row>
+    <row r="53" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P53" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q53" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P54" s="12">
+        <v>2025</v>
+      </c>
+      <c r="Q54" s="13">
+        <v>471000</v>
+      </c>
+    </row>
+    <row r="55" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P55" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q55" s="10">
+        <v>471000</v>
+      </c>
+    </row>
+    <row r="56" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P56" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q56" s="16">
+        <v>471000</v>
+      </c>
+    </row>
+    <row r="66" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G66" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H66" s="8"/>
+      <c r="I66" s="8"/>
+      <c r="J66" s="8"/>
+      <c r="K66" s="8"/>
+      <c r="L66" s="8"/>
+    </row>
+    <row r="67" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G67" s="8"/>
+      <c r="H67" s="8"/>
+      <c r="I67" s="8"/>
+      <c r="J67" s="8"/>
+      <c r="K67" s="8"/>
+      <c r="L67" s="8"/>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A47:E48"/>
+    <mergeCell ref="G47:L48"/>
+    <mergeCell ref="N47:S48"/>
+    <mergeCell ref="G66:L67"/>
+  </mergeCells>
+  <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId4"/>
   <extLst>

</xml_diff>